<commit_message>
Entitäten überarbeitet, Excel Doku überarbeitet
</commit_message>
<xml_diff>
--- a/EliteGaertner/docs/Datenmodell.xlsx
+++ b/EliteGaertner/docs/Datenmodell.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandarcvijic/Library/Mobile Documents/com~apple~CloudDocs/Dokumente/Studium/Module/Software Development Basics/RiderProjects/Projektarbeit/spassgetraenk/EliteGaertner/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3F766AC-BE1A-F543-84D6-54677A66C844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CC5B30-7AAD-1F4C-B732-1093E428C35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="21660" xr2:uid="{022C5B9C-E61A-7948-9E61-50C9903F8F3D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
   <si>
     <t>userName: string</t>
   </si>
@@ -56,9 +56,6 @@
     <t>profileText: string</t>
   </si>
   <si>
-    <t>userId: int (PK)</t>
-  </si>
-  <si>
     <t>uploadId: int (PK)</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>weightKg: float</t>
   </si>
   <si>
-    <t>uploadDate: date</t>
-  </si>
-  <si>
     <t>label: String</t>
   </si>
   <si>
@@ -104,15 +98,6 @@
     <t>Tomaten</t>
   </si>
   <si>
-    <t xml:space="preserve">preferenceId: int </t>
-  </si>
-  <si>
-    <t>userId1: int (PK)</t>
-  </si>
-  <si>
-    <t>userId2: int (PK)</t>
-  </si>
-  <si>
     <t>userIdRating: bool</t>
   </si>
   <si>
@@ -122,9 +107,6 @@
     <t>Timo</t>
   </si>
   <si>
-    <t xml:space="preserve">Timo </t>
-  </si>
-  <si>
     <t>Report</t>
   </si>
   <si>
@@ -146,18 +128,6 @@
     <t>05.12.2025</t>
   </si>
   <si>
-    <t>User.userId: int (RK)</t>
-  </si>
-  <si>
-    <t>02.12.2021</t>
-  </si>
-  <si>
-    <t>04.04.2024</t>
-  </si>
-  <si>
-    <t>01.12.2025</t>
-  </si>
-  <si>
     <t>…..</t>
   </si>
   <si>
@@ -194,24 +164,15 @@
     <t>04.12.2025</t>
   </si>
   <si>
-    <t>PREFERENCES</t>
-  </si>
-  <si>
     <t>HARVESTUPLOADS</t>
   </si>
   <si>
-    <t>USER</t>
-  </si>
-  <si>
     <t>TAGS</t>
   </si>
   <si>
     <t>TAGS.tagID: Int (RK)</t>
   </si>
   <si>
-    <t>USER.userID (RK)</t>
-  </si>
-  <si>
     <t>Jonas</t>
   </si>
   <si>
@@ -219,6 +180,69 @@
   </si>
   <si>
     <t>Kirchenbaur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1002 (Timo) </t>
+  </si>
+  <si>
+    <t>1001 (Aleks)</t>
+  </si>
+  <si>
+    <t>matchActive: bool</t>
+  </si>
+  <si>
+    <t>phoneNumber: int</t>
+  </si>
+  <si>
+    <t>shareMail: bool</t>
+  </si>
+  <si>
+    <t>sharePhoneNumber: bool</t>
+  </si>
+  <si>
+    <t>userCreated: DateTime</t>
+  </si>
+  <si>
+    <t>profileId: int (PK)</t>
+  </si>
+  <si>
+    <t>Profile.ProfileId: int (RK)</t>
+  </si>
+  <si>
+    <t>Dateupdated: DateTime</t>
+  </si>
+  <si>
+    <t>matchActiveDate: DateTime</t>
+  </si>
+  <si>
+    <t>ProfileId1: int (PK)</t>
+  </si>
+  <si>
+    <t>ProfileId2: int (PK)</t>
+  </si>
+  <si>
+    <t>PROFILE</t>
+  </si>
+  <si>
+    <t>PROFILEPREFERENCES</t>
+  </si>
+  <si>
+    <t>HARVESTTAGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAGS.tagID </t>
+  </si>
+  <si>
+    <t>preferenceId: int (PK)</t>
+  </si>
+  <si>
+    <t>HARVESTUPLOADS.uploadId: int (FK)</t>
+  </si>
+  <si>
+    <t>USER.userID (FK)</t>
+  </si>
+  <si>
+    <t>harvestTagId: int (PK)</t>
   </si>
 </sst>
 </file>
@@ -256,15 +280,57 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -309,7 +375,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -321,10 +387,10 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -333,102 +399,48 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -523,19 +535,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="double">
         <color indexed="64"/>
       </bottom>
@@ -550,6 +549,43 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -558,33 +594,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -919,494 +976,624 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B4F298D-41EF-1647-867E-DEEF723344D6}">
-  <dimension ref="A2:J50"/>
+  <dimension ref="A2:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="112" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:10" ht="23" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="24" t="s">
+    <row r="2" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:12" ht="23" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="L3" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="13"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="14">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B4" s="30">
         <v>1001</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="4">
+      <c r="C4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="10"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B5" s="35">
         <v>1002</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="4">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B6" s="2">
         <v>1003</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="4"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B7" s="2"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="4"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B8" s="2"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:10" ht="23" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="17" t="s">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="6"/>
+    </row>
+    <row r="11" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:12" ht="23" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="J12" s="21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="14">
+      <c r="F12" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B13" s="8">
         <v>2001</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15">
+      <c r="C13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9">
         <v>12</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="16">
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="31">
         <v>1001</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="4">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B14" s="2">
         <v>2002</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1">
+        <v>32</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1">
         <v>4</v>
       </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="5">
+      <c r="I14" s="34">
         <v>1002</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="4">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B15" s="28">
         <v>2003</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1">
+        <v>30</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1">
         <v>2</v>
       </c>
+      <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="5">
+      <c r="I15" s="29">
         <v>1001</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="4"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B16" s="2"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="5"/>
+      <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="4"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="5"/>
+      <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="8"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="6"/>
     </row>
     <row r="20" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:10" ht="23" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="25" t="s">
-        <v>52</v>
+      <c r="A21" s="18" t="s">
+        <v>62</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>57</v>
       </c>
+      <c r="D21" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="4">
+      <c r="B22" s="8">
         <v>3001</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="22"/>
+      <c r="D22" s="45">
         <v>5001</v>
       </c>
-      <c r="D22" s="5">
+      <c r="E22" s="31">
         <v>1001</v>
       </c>
+      <c r="H22" s="8">
+        <v>6001</v>
+      </c>
+      <c r="I22" s="9">
+        <v>5001</v>
+      </c>
+      <c r="J22" s="10">
+        <v>2001</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="4">
+      <c r="B23" s="2">
         <v>3002</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="19"/>
+      <c r="D23" s="46">
         <v>5002</v>
       </c>
-      <c r="D23" s="5">
+      <c r="E23" s="29">
         <v>1001</v>
       </c>
+      <c r="H23" s="2">
+        <v>6002</v>
+      </c>
+      <c r="I23" s="1">
+        <v>5002</v>
+      </c>
+      <c r="J23" s="3">
+        <v>2001</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B24" s="4">
+      <c r="B24" s="2">
         <v>3003</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="19"/>
+      <c r="D24" s="44">
         <v>5001</v>
       </c>
-      <c r="D24" s="5">
+      <c r="E24" s="34">
         <v>1002</v>
       </c>
+      <c r="H24" s="2"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="3"/>
     </row>
     <row r="25" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="6">
+      <c r="B25" s="4">
         <v>3004</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="20"/>
+      <c r="D25" s="43">
         <v>5003</v>
       </c>
-      <c r="D25" s="8">
+      <c r="E25" s="37">
         <v>1002</v>
       </c>
+      <c r="H25" s="4"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="6"/>
     </row>
     <row r="29" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:10" ht="23" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="24" t="s">
+      <c r="A30" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J30" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B31" s="40">
+        <v>5001</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="8">
+        <v>4001</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G30" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="H30" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="I30" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="J30" s="19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B31" s="4">
-        <v>5001</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" s="14">
-        <v>4001</v>
-      </c>
-      <c r="H31" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I31" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="J31" s="16">
+      <c r="J31" s="26">
         <v>2003</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B32" s="4">
+      <c r="B32" s="41">
         <v>5002</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G32" s="4">
+      <c r="C32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="2">
         <v>4002</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J32" s="5">
+        <v>41</v>
+      </c>
+      <c r="J32" s="27">
         <v>2003</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B33" s="4">
+      <c r="B33" s="42">
         <v>5003</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G33" s="4"/>
+      <c r="C33" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" s="2"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="5"/>
+      <c r="J33" s="3"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="4"/>
-      <c r="C34" s="5"/>
-      <c r="G34" s="4"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="3"/>
+      <c r="G34" s="2"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="5"/>
+      <c r="J34" s="3"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B35" s="4"/>
-      <c r="C35" s="5"/>
-      <c r="G35" s="4"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="3"/>
+      <c r="G35" s="2"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="5"/>
+      <c r="J35" s="3"/>
     </row>
     <row r="36" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="6"/>
-      <c r="C36" s="8"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="8"/>
-    </row>
-    <row r="39" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="s">
+      <c r="B36" s="4"/>
+      <c r="C36" s="6"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="6"/>
+    </row>
+    <row r="38" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:10" ht="23" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="E39" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B40" s="23">
+        <v>567</v>
+      </c>
+      <c r="C40" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="E40" s="9"/>
+      <c r="F40" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B41" s="2"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B42" s="2"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B43" s="2"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B44" s="2"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="4"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="6"/>
+    </row>
+    <row r="47" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:10" ht="23" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C39" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B40">
+      <c r="F48" s="7"/>
+      <c r="H48" s="7"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B49" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" s="9">
+        <v>1</v>
+      </c>
+      <c r="E49" s="24">
         <v>567</v>
       </c>
-      <c r="C40" t="s">
-        <v>28</v>
-      </c>
-      <c r="D40" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A48" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D48" t="s">
-        <v>25</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F48" s="12"/>
-      <c r="H48" s="12"/>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
-        <v>26</v>
-      </c>
-      <c r="C49" t="s">
-        <v>27</v>
-      </c>
-      <c r="D49">
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B50" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50" s="1">
         <v>1</v>
       </c>
-      <c r="E49">
+      <c r="E50" s="25">
         <v>567</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
-        <v>27</v>
-      </c>
-      <c r="C50" t="s">
-        <v>26</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="E50">
-        <v>567</v>
-      </c>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B51" s="2"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B52" s="2"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="4"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Datebankonzept finalisiert und Entitäten überarbeitet, weiter am Vorschlagsalgorithmus gearbeitet
</commit_message>
<xml_diff>
--- a/EliteGaertner/docs/Datenmodell.xlsx
+++ b/EliteGaertner/docs/Datenmodell.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandarcvijic/Library/Mobile Documents/com~apple~CloudDocs/Dokumente/Studium/Module/Software Development Basics/RiderProjects/Projektarbeit/spassgetraenk/EliteGaertner/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CC5B30-7AAD-1F4C-B732-1093E428C35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CE7154-FCC1-454D-B0E4-12139FAD1C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="21660" xr2:uid="{022C5B9C-E61A-7948-9E61-50C9903F8F3D}"/>
+    <workbookView xWindow="17280" yWindow="680" windowWidth="17280" windowHeight="21660" xr2:uid="{022C5B9C-E61A-7948-9E61-50C9903F8F3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
   <si>
     <t>userName: string</t>
   </si>
@@ -74,33 +74,15 @@
     <t>tagId: int (PK)</t>
   </si>
   <si>
-    <t>Matches</t>
-  </si>
-  <si>
-    <t>userId1</t>
-  </si>
-  <si>
-    <t>userId2</t>
-  </si>
-  <si>
-    <t>matchID: int (PK)</t>
-  </si>
-  <si>
     <t>Rating</t>
   </si>
   <si>
-    <t>matchId: int (RK)</t>
-  </si>
-  <si>
     <t>Biologisch angebaut</t>
   </si>
   <si>
     <t>Tomaten</t>
   </si>
   <si>
-    <t>userIdRating: bool</t>
-  </si>
-  <si>
     <t>Aleks</t>
   </si>
   <si>
@@ -134,9 +116,6 @@
     <t>….</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
     <t>lengthCm: float</t>
   </si>
   <si>
@@ -170,9 +149,6 @@
     <t>TAGS</t>
   </si>
   <si>
-    <t>TAGS.tagID: Int (RK)</t>
-  </si>
-  <si>
     <t>Jonas</t>
   </si>
   <si>
@@ -188,12 +164,6 @@
     <t>1001 (Aleks)</t>
   </si>
   <si>
-    <t>matchActive: bool</t>
-  </si>
-  <si>
-    <t>phoneNumber: int</t>
-  </si>
-  <si>
     <t>shareMail: bool</t>
   </si>
   <si>
@@ -206,21 +176,12 @@
     <t>profileId: int (PK)</t>
   </si>
   <si>
-    <t>Profile.ProfileId: int (RK)</t>
-  </si>
-  <si>
     <t>Dateupdated: DateTime</t>
   </si>
   <si>
     <t>matchActiveDate: DateTime</t>
   </si>
   <si>
-    <t>ProfileId1: int (PK)</t>
-  </si>
-  <si>
-    <t>ProfileId2: int (PK)</t>
-  </si>
-  <si>
     <t>PROFILE</t>
   </si>
   <si>
@@ -230,19 +191,34 @@
     <t>HARVESTTAGS</t>
   </si>
   <si>
-    <t xml:space="preserve">TAGS.tagID </t>
-  </si>
-  <si>
-    <t>preferenceId: int (PK)</t>
-  </si>
-  <si>
-    <t>HARVESTUPLOADS.uploadId: int (FK)</t>
-  </si>
-  <si>
-    <t>USER.userID (FK)</t>
-  </si>
-  <si>
-    <t>harvestTagId: int (PK)</t>
+    <t>ratingDate: DateTime</t>
+  </si>
+  <si>
+    <t>profile Rating: bool</t>
+  </si>
+  <si>
+    <t>phoneNumber: string</t>
+  </si>
+  <si>
+    <t>Profile.ProfileId: int (FK)</t>
+  </si>
+  <si>
+    <t>TAGS.tagID (PK, FK)</t>
+  </si>
+  <si>
+    <t>HARVESTUPLOADS.uploadId: int (PK, FK)</t>
+  </si>
+  <si>
+    <t>TAGS.tagID: Int (PK, FK)</t>
+  </si>
+  <si>
+    <t>contentCreator: int (PK)</t>
+  </si>
+  <si>
+    <t>contentReceiver: int (PK)</t>
+  </si>
+  <si>
+    <t>PROFILE.profileID (PK, FK)</t>
   </si>
 </sst>
 </file>
@@ -280,7 +256,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,12 +266,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -555,7 +525,18 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -568,24 +549,13 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -594,7 +564,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -614,34 +584,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -976,24 +939,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B4F298D-41EF-1647-867E-DEEF723344D6}">
-  <dimension ref="A2:L53"/>
+  <dimension ref="A2:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="112" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="33.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1001,10 +961,10 @@
     <row r="2" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:12" ht="23" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>0</v>
@@ -1022,33 +982,33 @@
         <v>4</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I3" s="12" t="s">
         <v>5</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="L3" s="39" t="s">
-        <v>54</v>
+        <v>42</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="30">
+      <c r="B4" s="24">
         <v>1001</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -1059,17 +1019,17 @@
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="35">
+      <c r="B5" s="28">
         <v>1002</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1084,13 +1044,13 @@
         <v>1003</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -1142,7 +1102,7 @@
     <row r="11" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:12" ht="23" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>6</v>
@@ -1157,16 +1117,16 @@
         <v>9</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1174,7 +1134,7 @@
         <v>2001</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9">
@@ -1183,7 +1143,7 @@
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
-      <c r="I13" s="31">
+      <c r="I13" s="25">
         <v>1001</v>
       </c>
     </row>
@@ -1192,7 +1152,7 @@
         <v>2002</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1">
@@ -1201,16 +1161,16 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="34">
+      <c r="I14" s="27">
         <v>1002</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B15" s="28">
+      <c r="B15" s="22">
         <v>2003</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1">
@@ -1219,7 +1179,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="29">
+      <c r="I15" s="23">
         <v>1001</v>
       </c>
     </row>
@@ -1256,109 +1216,83 @@
     <row r="20" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:10" ht="23" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="I21" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="J21" s="13" t="s">
-        <v>66</v>
+      <c r="C21" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" s="34" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="8">
-        <v>3001</v>
-      </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="45">
+      <c r="B22" s="31">
         <v>5001</v>
       </c>
-      <c r="E22" s="31">
+      <c r="C22" s="25">
         <v>1001</v>
       </c>
-      <c r="H22" s="8">
-        <v>6001</v>
-      </c>
-      <c r="I22" s="9">
+      <c r="D22" s="35"/>
+      <c r="G22" s="9">
         <v>5001</v>
       </c>
-      <c r="J22" s="10">
+      <c r="H22" s="10">
         <v>2001</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="2">
-        <v>3002</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="46">
+      <c r="B23" s="32">
         <v>5002</v>
       </c>
-      <c r="E23" s="29">
+      <c r="C23" s="23">
         <v>1001</v>
       </c>
-      <c r="H23" s="2">
-        <v>6002</v>
-      </c>
-      <c r="I23" s="1">
+      <c r="D23" s="36"/>
+      <c r="G23" s="1">
         <v>5002</v>
       </c>
-      <c r="J23" s="3">
+      <c r="H23" s="3">
         <v>2001</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B24" s="2">
-        <v>3003</v>
-      </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="44">
+      <c r="B24" s="37">
         <v>5001</v>
       </c>
-      <c r="E24" s="34">
+      <c r="C24" s="27">
         <v>1002</v>
       </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="3"/>
+      <c r="D24" s="36"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="4">
-        <v>3004</v>
-      </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="43">
+      <c r="B25" s="38">
         <v>5003</v>
       </c>
-      <c r="E25" s="37">
+      <c r="C25" s="30">
         <v>1002</v>
       </c>
-      <c r="H25" s="4"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="6"/>
+      <c r="D25" s="39"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="6"/>
     </row>
     <row r="29" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:10" ht="23" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="17" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>11</v>
@@ -1367,67 +1301,67 @@
         <v>10</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B31" s="40">
+      <c r="B31" s="31">
         <v>5001</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G31" s="8">
         <v>4001</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J31" s="26">
+        <v>23</v>
+      </c>
+      <c r="J31" s="20">
         <v>2003</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B32" s="41">
+      <c r="B32" s="32">
         <v>5002</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G32" s="2">
         <v>4002</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J32" s="27">
+        <v>34</v>
+      </c>
+      <c r="J32" s="21">
         <v>2003</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B33" s="42">
+      <c r="B33" s="33">
         <v>5003</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="1"/>
@@ -1458,142 +1392,69 @@
       <c r="I36" s="5"/>
       <c r="J36" s="6"/>
     </row>
-    <row r="38" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:10" ht="23" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="17" t="s">
+    <row r="40" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:10" ht="23" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E39" s="12" t="s">
+      <c r="B41" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F39" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B40" s="23">
-        <v>567</v>
-      </c>
-      <c r="C40" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="D40" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="E40" s="9"/>
-      <c r="F40" s="10" t="b">
+      <c r="C41" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H41" s="7"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B42" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B41" s="2"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B42" s="2"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="3"/>
+      <c r="E42" s="10"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B43" s="2"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="3"/>
+      <c r="B43" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1</v>
+      </c>
+      <c r="E43" s="3"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B44" s="2"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="4"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="6"/>
-    </row>
-    <row r="47" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:10" ht="23" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C48" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F48" s="7"/>
-      <c r="H48" s="7"/>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B49" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="C49" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="D49" s="9">
-        <v>1</v>
-      </c>
-      <c r="E49" s="24">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B50" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="C50" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="D50" s="1">
-        <v>1</v>
-      </c>
-      <c r="E50" s="25">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B51" s="2"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="3"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B52" s="2"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="3"/>
-    </row>
-    <row r="53" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="4"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="6"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B45" s="2"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="4"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>